<commit_message>
Fix for malformed board at baby stop tile
</commit_message>
<xml_diff>
--- a/utils/boardLayout/layout.xlsx
+++ b/utils/boardLayout/layout.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Mannion\Google Drive\Stage 5\Software Engineering\Project\boardLayout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Mannion\Google Drive\Stage 5\Software Engineering\Project\utils\boardLayout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A70D1AC-DCC1-4862-BDA5-B40C33B424FD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96DE428-A734-4A95-B72B-B01F14A4E102}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1872" yWindow="0" windowWidth="16560" windowHeight="6120" xr2:uid="{A600518B-26ED-4E34-8A0B-01D17C55EABF}"/>
+    <workbookView xWindow="2808" yWindow="0" windowWidth="16560" windowHeight="6120" xr2:uid="{A600518B-26ED-4E34-8A0B-01D17C55EABF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="134">
   <si>
     <t>Payday</t>
   </si>
@@ -178,9 +177,6 @@
     <t>14,10,1,0.5</t>
   </si>
   <si>
-    <t>17,10,1,0.5</t>
-  </si>
-  <si>
     <t>3,11,1,0.5</t>
   </si>
   <si>
@@ -262,9 +258,6 @@
     <t>9,9,1,0.5</t>
   </si>
   <si>
-    <t>17,9,1,0.5</t>
-  </si>
-  <si>
     <t>7,8,1,0.5</t>
   </si>
   <si>
@@ -437,6 +430,9 @@
   </si>
   <si>
     <t>15,-6,2,5</t>
+  </si>
+  <si>
+    <t>17,9,1,1</t>
   </si>
 </sst>
 </file>
@@ -508,7 +504,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -656,11 +652,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -696,6 +701,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1012,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADD7C30-E0A9-454A-9297-230E452D259A}">
   <dimension ref="A1:AB128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1051,7 +1058,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -1089,7 +1096,7 @@
         <v>33</v>
       </c>
       <c r="Y10" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Z10" s="24"/>
     </row>
@@ -1105,19 +1112,19 @@
         <v>31</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="W12" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="X12" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Y12" s="25"/>
       <c r="Z12" s="26"/>
@@ -1127,7 +1134,7 @@
         <v>30</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Y13" s="25"/>
       <c r="Z13" s="26"/>
@@ -1137,7 +1144,7 @@
         <v>25</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="Y14" s="27"/>
       <c r="Z14" s="28"/>
@@ -1147,7 +1154,7 @@
         <v>29</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
@@ -1158,16 +1165,16 @@
         <v>3</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="V16" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="W16" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W16" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="X16" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.3">
@@ -1175,13 +1182,13 @@
         <v>27</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="V17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="X17" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="X17" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
@@ -1189,25 +1196,25 @@
         <v>26</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="V18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y18" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="X18" s="2" t="s">
+      <c r="Z18" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="Y18" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z18" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="AA18" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
@@ -1215,7 +1222,7 @@
         <v>40</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.3">
@@ -1223,7 +1230,7 @@
         <v>41</v>
       </c>
       <c r="AA20" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.3">
@@ -1231,25 +1238,25 @@
         <v>22</v>
       </c>
       <c r="U21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="V21" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="V21" s="2" t="s">
+      <c r="W21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="X21" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="W21" s="2" t="s">
+      <c r="Y21" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="X21" s="2" t="s">
+      <c r="Z21" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="Y21" s="2" t="s">
+      <c r="AA21" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="Z21" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AA21" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.3">
@@ -1257,7 +1264,7 @@
         <v>21</v>
       </c>
       <c r="U22" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.3">
@@ -1265,22 +1272,22 @@
         <v>20</v>
       </c>
       <c r="M23" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="N23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="P23" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="Q23" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="P23" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="U23" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.3">
@@ -1289,34 +1296,34 @@
       </c>
       <c r="M24" s="16"/>
       <c r="Q24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="S24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="R24" s="2" t="s">
+      <c r="U24" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="S24" s="2" t="s">
+      <c r="V24" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="U24" s="12" t="s">
+      <c r="W24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="V24" s="2" t="s">
+      <c r="X24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="W24" s="2" t="s">
+      <c r="Y24" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="X24" s="2" t="s">
+      <c r="Z24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="Y24" s="2" t="s">
+      <c r="AA24" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="Z24" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA24" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.3">
@@ -1324,16 +1331,16 @@
         <v>18</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q25" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA25" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="AA25" s="32" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.3">
@@ -1344,7 +1351,7 @@
         <v>4</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L26" s="6"/>
       <c r="M26" s="13" t="s">
@@ -1367,12 +1374,10 @@
         <v>47</v>
       </c>
       <c r="Y26" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Z26" s="6"/>
-      <c r="AA26" s="13" t="s">
-        <v>48</v>
-      </c>
+      <c r="AA26" s="31"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
@@ -1382,19 +1387,19 @@
         <v>5</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q27" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="S27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="U27" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="U27" s="2" t="s">
+      <c r="AA27" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="AA27" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.3">
@@ -1405,17 +1410,17 @@
         <v>6</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q28" s="16"/>
       <c r="S28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="U28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="U28" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="AA28" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.3">
@@ -1426,43 +1431,43 @@
         <v>7</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O29" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O29" s="2" t="s">
+      <c r="P29" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="P29" s="12" t="s">
+      <c r="Q29" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="Q29" s="2" t="s">
+      <c r="S29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="S29" s="2" t="s">
+      <c r="U29" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="U29" s="13" t="s">
+      <c r="V29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V29" s="2" t="s">
+      <c r="W29" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="W29" s="2" t="s">
+      <c r="X29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="X29" s="2" t="s">
+      <c r="Y29" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Y29" s="2" t="s">
+      <c r="Z29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Z29" s="2" t="s">
+      <c r="AA29" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="AA29" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.3">
@@ -1473,10 +1478,10 @@
         <v>8</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U30" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.3">
@@ -1487,13 +1492,13 @@
         <v>9</v>
       </c>
       <c r="S31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="T31" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="T31" s="2" t="s">
+      <c r="U31" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="U31" s="12" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.3">
@@ -1619,7 +1624,7 @@
       </c>
       <c r="W37" s="8"/>
       <c r="X37" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Y37" s="5"/>
       <c r="Z37" s="30" t="s">
@@ -1644,7 +1649,7 @@
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.3">
@@ -1653,12 +1658,12 @@
       </c>
       <c r="E41" s="29"/>
       <c r="F41" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" t="s">
@@ -1667,7 +1672,7 @@
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" t="s">
@@ -1676,7 +1681,7 @@
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E44" s="14"/>
       <c r="F44" t="s">
@@ -1685,90 +1690,90 @@
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
@@ -1778,57 +1783,57 @@
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
@@ -1853,102 +1858,102 @@
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
-        <v>81</v>
+      <c r="A93" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="12" t="s">
-        <v>80</v>
+      <c r="A94" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="11" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
@@ -1958,62 +1963,62 @@
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="2" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="12" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
@@ -2023,92 +2028,92 @@
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
-        <v>107</v>
+      <c r="A112" s="12" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" s="12" t="s">
-        <v>105</v>
+      <c r="A113" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
-        <v>130</v>
+      <c r="A118" s="12" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119" s="12" t="s">
-        <v>131</v>
+      <c r="A119" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" s="2" t="s">
-        <v>129</v>
+      <c r="A125" s="6" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" s="23" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" s="6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Overall use case diagram, UML diagrams updated after refactoring
</commit_message>
<xml_diff>
--- a/utils/boardLayout/layout.xlsx
+++ b/utils/boardLayout/layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Mannion\Google Drive\Stage 5\Software Engineering\Project\utils\boardLayout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96DE428-A734-4A95-B72B-B01F14A4E102}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29162D1A-B7A0-4763-8164-608834B5D532}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2808" yWindow="0" windowWidth="16560" windowHeight="6120" xr2:uid="{A600518B-26ED-4E34-8A0B-01D17C55EABF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="134">
   <si>
     <t>Payday</t>
   </si>
@@ -1017,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADD7C30-E0A9-454A-9297-230E452D259A}">
-  <dimension ref="A1:AB128"/>
+  <dimension ref="A1:AB127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2111,11 +2111,6 @@
         <v>132</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" s="23" t="s">
-        <v>132</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>